<commit_message>
Formato Libro Compras Corregido
</commit_message>
<xml_diff>
--- a/app/templates/contable/plantillas/Registro_Compras.xlsx
+++ b/app/templates/contable/plantillas/Registro_Compras.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis.DESKTOP-CH6GAAE\Desktop\LUIS\SEMESTRE 2024-II\CALIDAD\PROYECTO\GITHUB\CONTABILIDAD_PROYECTO\app\templates\contable\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamir\OneDrive\Documentos\Visual Studio Code\CONTABILIDAD_PROYECTO\app\templates\contable\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0528FDA-03B5-496E-93BD-CB56D3728B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0115B08F-9234-4C82-A109-CA2A22CA8D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="809" xr2:uid="{562E8E1C-C923-4D87-B52B-9A6EFD03C8D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="809" xr2:uid="{562E8E1C-C923-4D87-B52B-9A6EFD03C8D5}"/>
   </bookViews>
   <sheets>
     <sheet name="F 8.1 Registro de Compras" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'F 8.1 Registro de Compras'!$A$1:$M$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'F 8.1 Registro de Compras'!$A$1:$M$20</definedName>
     <definedName name="VENCII">[1]CRONOGRAMA!$C$83:$D$452</definedName>
   </definedNames>
   <calcPr calcId="92512"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>PERIODO:</t>
   </si>
@@ -47,19 +47,7 @@
     <t>APELLIDOS Y NOMBRES, DENOMINACIÓN O RAZÓN SOCIAL:</t>
   </si>
   <si>
-    <t>(2) Sólo para los casos de utilización de servicios o adquisiciones de intangibles provenientes del exterior.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3) Sólo para los casos de detracciones. Es optativo el llenado cuando exista un sistema de enlace que mantenga dicha información y se pueda identificar los comprobantes de pago respecto de los cuales se efectuó el depósito. </t>
-  </si>
-  <si>
-    <t>(1) Señalar la fecha correspondiente, de acuerdo a lo establecido en el literal b) del inciso II del numeral 1 del Articulo 10 del Reglamento de la Ley del IGV.</t>
-  </si>
-  <si>
     <t>IMPORTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  TOTAL</t>
   </si>
   <si>
     <t>REGISTRO DE COMPRAS</t>
@@ -111,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ [$€]* #,##0.00_ ;_ [$€]* \-#,##0.00_ ;_ [$€]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -119,6 +107,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -128,6 +117,7 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -149,20 +139,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -196,12 +172,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -323,21 +299,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -347,67 +314,54 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3450,9 +3404,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3490,7 +3444,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3596,7 +3550,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3738,7 +3692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3746,541 +3700,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3925FA87-9B1D-476F-9E4A-BD8A040B7CD3}">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="32.109375" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1"/>
-    <col min="7" max="7" width="49.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="49.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" customWidth="1"/>
-    <col min="11" max="11" width="35.88671875" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" customWidth="1"/>
-    <col min="13" max="13" width="35.6640625" customWidth="1"/>
-    <col min="14" max="14" width="32.33203125" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" customWidth="1"/>
+    <col min="11" max="11" width="35.85546875" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" customWidth="1"/>
+    <col min="13" max="13" width="35.7109375" customWidth="1"/>
+    <col min="14" max="14" width="32.28515625" customWidth="1"/>
     <col min="15" max="15" width="35" customWidth="1"/>
-    <col min="16" max="16" width="26.6640625" customWidth="1"/>
-    <col min="17" max="17" width="20.109375" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" customWidth="1"/>
-    <col min="19" max="19" width="18.88671875" customWidth="1"/>
-    <col min="20" max="20" width="18.5546875" customWidth="1"/>
-    <col min="21" max="21" width="24.6640625" customWidth="1"/>
-    <col min="22" max="23" width="18.5546875" customWidth="1"/>
-    <col min="28" max="28" width="20.44140625" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" customWidth="1"/>
+    <col min="21" max="21" width="24.7109375" customWidth="1"/>
+    <col min="22" max="23" width="18.5703125" customWidth="1"/>
+    <col min="28" max="28" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:13" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="18"/>
+    </row>
+    <row r="9" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="E9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="F9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>15</v>
+      <c r="G9" s="15"/>
+      <c r="H9" s="20" t="s">
+        <v>4</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="21" t="s">
-        <v>19</v>
+      <c r="I9" s="21"/>
+      <c r="J9" s="14" t="s">
+        <v>18</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="K9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="17" t="s">
-        <v>23</v>
+      <c r="L9" s="14" t="s">
+        <v>3</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="12"/>
+      <c r="M9" s="18"/>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="21" t="s">
+    <row r="10" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="13"/>
+    <row r="11" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="11"/>
+    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="9"/>
+    <row r="13" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+    <row r="17" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
+    <row r="18" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="14"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
+    <row r="19" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="7"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="14"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="14"/>
-      <c r="AB20" s="14"/>
-    </row>
-    <row r="21" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="14"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="14"/>
-      <c r="Z21" s="14"/>
-      <c r="AA21" s="14"/>
-      <c r="AB21" s="14"/>
-    </row>
-    <row r="22" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="14"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="14"/>
-      <c r="AA22" s="14"/>
-      <c r="AB22" s="14"/>
-    </row>
-    <row r="23" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="14"/>
-      <c r="Z23" s="14"/>
-      <c r="AA23" s="14"/>
-      <c r="AB23" s="14"/>
-    </row>
-    <row r="24" spans="1:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
-      <c r="Z24" s="14"/>
-      <c r="AA24" s="14"/>
-      <c r="AB24" s="14"/>
-    </row>
-    <row r="25" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-    </row>
-    <row r="26" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-    </row>
-    <row r="27" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-    </row>
-    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+    <row r="20" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="7"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="H9:I9"/>
+  <mergeCells count="17">
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="B7:B13"/>
     <mergeCell ref="C7:C13"/>
@@ -4290,12 +4044,14 @@
     <mergeCell ref="L9:L13"/>
     <mergeCell ref="D9:D13"/>
     <mergeCell ref="E9:E13"/>
+    <mergeCell ref="M7:M13"/>
     <mergeCell ref="F9:F13"/>
     <mergeCell ref="G7:G13"/>
     <mergeCell ref="H7:J8"/>
     <mergeCell ref="H10:H13"/>
     <mergeCell ref="I10:I13"/>
     <mergeCell ref="J9:J13"/>
+    <mergeCell ref="H9:I9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>